<commit_message>
management aircraft flown twice in the same base. ultimate version of the function
</commit_message>
<xml_diff>
--- a/FH-task2/FH_bases_ultimateBASE1_pafam_optimization_results.xlsx
+++ b/FH-task2/FH_bases_ultimateBASE1_pafam_optimization_results.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="76">
   <si>
     <t>FH init</t>
   </si>
@@ -115,6 +115,9 @@
     <t>AT005</t>
   </si>
   <si>
+    <t>88, 267</t>
+  </si>
+  <si>
     <t>AC</t>
   </si>
   <si>
@@ -133,91 +136,94 @@
     <t>ISO3_D3-B11</t>
   </si>
   <si>
+    <t>178, 422</t>
+  </si>
+  <si>
     <t xml:space="preserve">base_1 </t>
   </si>
   <si>
+    <t xml:space="preserve">base_2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BASE 0 </t>
+  </si>
+  <si>
+    <t>2024</t>
+  </si>
+  <si>
+    <t>Total FH flown in this base</t>
+  </si>
+  <si>
+    <t>Total FH flown AC</t>
+  </si>
+  <si>
+    <t>Total FH flown AT</t>
+  </si>
+  <si>
+    <t>AC006</t>
+  </si>
+  <si>
+    <t>AC008</t>
+  </si>
+  <si>
+    <t>AC013</t>
+  </si>
+  <si>
+    <t>AC017</t>
+  </si>
+  <si>
+    <t>AC019</t>
+  </si>
+  <si>
+    <t>AT004</t>
+  </si>
+  <si>
+    <t>1780, 1850</t>
+  </si>
+  <si>
+    <t>ISO3_D3-B8</t>
+  </si>
+  <si>
+    <t>D3-B2</t>
+  </si>
+  <si>
+    <t>ISO2_E-B8</t>
+  </si>
+  <si>
+    <t>ISO4_F-B2</t>
+  </si>
+  <si>
+    <t>1850, 1910</t>
+  </si>
+  <si>
+    <t xml:space="preserve">base_0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BASE 1 </t>
+  </si>
+  <si>
+    <t>AC004</t>
+  </si>
+  <si>
+    <t>AC009</t>
+  </si>
+  <si>
+    <t>AC011</t>
+  </si>
+  <si>
+    <t>ISO2_E-B9</t>
+  </si>
+  <si>
+    <t>ISO4_F-B6</t>
+  </si>
+  <si>
+    <t>ISO1_D-B9</t>
+  </si>
+  <si>
+    <t>ISO3_D3-B3</t>
+  </si>
+  <si>
     <t xml:space="preserve">base_3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">base_2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BASE 0 </t>
-  </si>
-  <si>
-    <t>2024</t>
-  </si>
-  <si>
-    <t>Total FH flown in this base</t>
-  </si>
-  <si>
-    <t>Total FH flown AC</t>
-  </si>
-  <si>
-    <t>Total FH flown AT</t>
-  </si>
-  <si>
-    <t>AC006</t>
-  </si>
-  <si>
-    <t>AC008</t>
-  </si>
-  <si>
-    <t>AC013</t>
-  </si>
-  <si>
-    <t>AC017</t>
-  </si>
-  <si>
-    <t>AC019</t>
-  </si>
-  <si>
-    <t>AT004</t>
-  </si>
-  <si>
-    <t>1780, 1850</t>
-  </si>
-  <si>
-    <t>ISO3_D3-B8</t>
-  </si>
-  <si>
-    <t>D3-B2</t>
-  </si>
-  <si>
-    <t>ISO4_F-B6</t>
-  </si>
-  <si>
-    <t>ISO2_E-B8</t>
-  </si>
-  <si>
-    <t>ISO4_F-B2</t>
-  </si>
-  <si>
-    <t>1850, 1850</t>
-  </si>
-  <si>
-    <t xml:space="preserve">base_0 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BASE 1 </t>
-  </si>
-  <si>
-    <t>AC004</t>
-  </si>
-  <si>
-    <t>AC009</t>
-  </si>
-  <si>
-    <t>AC011</t>
-  </si>
-  <si>
-    <t>ISO2_E-B9</t>
-  </si>
-  <si>
-    <t>ISO1_D-B9</t>
-  </si>
-  <si>
-    <t>ISO3_D3-B3</t>
   </si>
   <si>
     <t xml:space="preserve">BASE 2 </t>
@@ -627,7 +633,7 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="G1" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -638,7 +644,7 @@
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2"/>
     </row>
@@ -705,11 +711,11 @@
       <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B4">
-        <v>88</v>
+      <c r="B4" t="s">
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D4">
         <v>30</v>
@@ -720,14 +726,14 @@
       <c r="F4">
         <v>30</v>
       </c>
-      <c r="G4">
-        <v>30</v>
-      </c>
-      <c r="H4">
-        <v>30</v>
-      </c>
-      <c r="I4">
-        <v>29</v>
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" t="s">
+        <v>35</v>
       </c>
       <c r="J4">
         <v>28</v>
@@ -735,29 +741,29 @@
       <c r="K4">
         <v>27</v>
       </c>
-      <c r="L4" t="s">
-        <v>34</v>
-      </c>
-      <c r="M4" t="s">
-        <v>34</v>
-      </c>
-      <c r="N4" t="s">
-        <v>34</v>
-      </c>
-      <c r="O4" t="s">
-        <v>34</v>
+      <c r="L4">
+        <v>27</v>
+      </c>
+      <c r="M4">
+        <v>26</v>
+      </c>
+      <c r="N4">
+        <v>24</v>
+      </c>
+      <c r="O4">
+        <v>23</v>
       </c>
       <c r="P4">
-        <v>234</v>
-      </c>
-      <c r="Q4">
-        <v>322</v>
+        <v>245</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>39</v>
       </c>
       <c r="R4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -768,7 +774,7 @@
         <v>135</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D5">
         <v>30</v>
@@ -795,16 +801,16 @@
         <v>30</v>
       </c>
       <c r="L5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="O5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P5">
         <v>240</v>
@@ -813,10 +819,10 @@
         <v>375</v>
       </c>
       <c r="R5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -827,31 +833,31 @@
         <v>913</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L6">
         <v>22</v>
@@ -872,10 +878,10 @@
         <v>995</v>
       </c>
       <c r="R6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="S6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -886,7 +892,7 @@
         <v>1219</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -931,10 +937,10 @@
         <v>1289</v>
       </c>
       <c r="R7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -945,7 +951,7 @@
         <v>1432</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D8">
         <v>11</v>
@@ -966,22 +972,22 @@
         <v>12</v>
       </c>
       <c r="J8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P8">
         <v>68</v>
@@ -990,10 +996,10 @@
         <v>1500</v>
       </c>
       <c r="R8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -1004,7 +1010,7 @@
         <v>1614</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D9">
         <v>10</v>
@@ -1022,25 +1028,25 @@
         <v>11</v>
       </c>
       <c r="I9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="O9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P9">
         <v>52</v>
@@ -1049,10 +1055,10 @@
         <v>1666</v>
       </c>
       <c r="R9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -1063,7 +1069,7 @@
         <v>1694</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D10">
         <v>12</v>
@@ -1108,10 +1114,10 @@
         <v>1833</v>
       </c>
       <c r="R10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:19">
@@ -1122,7 +1128,7 @@
         <v>1590</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D11">
         <v>6</v>
@@ -1167,10 +1173,10 @@
         <v>1672</v>
       </c>
       <c r="R11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -1181,7 +1187,7 @@
         <v>1940</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D12">
         <v>12</v>
@@ -1199,25 +1205,25 @@
         <v>12</v>
       </c>
       <c r="I12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="M12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P12">
         <v>60</v>
@@ -1226,10 +1232,10 @@
         <v>2000</v>
       </c>
       <c r="R12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:19">
@@ -1240,19 +1246,19 @@
         <v>2000</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H13">
         <v>27</v>
@@ -1285,10 +1291,10 @@
         <v>2185</v>
       </c>
       <c r="R13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:19">
@@ -1299,7 +1305,7 @@
         <v>1063</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D14">
         <v>5</v>
@@ -1344,10 +1350,10 @@
         <v>1131</v>
       </c>
       <c r="R14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:19">
@@ -1358,7 +1364,7 @@
         <v>1271</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D15">
         <v>16</v>
@@ -1403,10 +1409,10 @@
         <v>1453</v>
       </c>
       <c r="R15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:19">
@@ -1417,43 +1423,43 @@
         <v>2000</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="O16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P16">
         <v>0</v>
@@ -1462,27 +1468,26 @@
         <v>2000</v>
       </c>
       <c r="R16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S16" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="16:18">
       <c r="P18" s="4">
-        <f>SUM(P3:P16)</f>
-        <v>0</v>
+        <v>1473</v>
       </c>
       <c r="R18" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="16:18">
       <c r="P19" s="4">
-        <v>1212</v>
+        <v>1223</v>
       </c>
       <c r="R19" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="16:18">
@@ -1490,7 +1495,7 @@
         <v>250</v>
       </c>
       <c r="R20" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1504,7 +1509,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S15"/>
+  <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1523,7 +1528,7 @@
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2"/>
     </row>
@@ -1588,22 +1593,22 @@
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="3" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="B4">
-        <v>530</v>
+        <v>178</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4">
-        <v>30</v>
-      </c>
-      <c r="E4">
-        <v>30</v>
-      </c>
-      <c r="F4">
-        <v>30</v>
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" t="s">
+        <v>35</v>
       </c>
       <c r="G4">
         <v>30</v>
@@ -1612,155 +1617,155 @@
         <v>30</v>
       </c>
       <c r="I4">
-        <v>30</v>
-      </c>
-      <c r="J4">
-        <v>30</v>
-      </c>
-      <c r="K4">
-        <v>30</v>
-      </c>
-      <c r="L4">
-        <v>30</v>
-      </c>
-      <c r="M4">
-        <v>30</v>
-      </c>
-      <c r="N4">
-        <v>30</v>
-      </c>
-      <c r="O4">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="J4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" t="s">
+        <v>35</v>
+      </c>
+      <c r="O4" t="s">
+        <v>35</v>
       </c>
       <c r="P4">
-        <v>360</v>
+        <v>89</v>
       </c>
       <c r="Q4">
-        <v>890</v>
+        <v>267</v>
       </c>
       <c r="R4" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="S4" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="B5">
-        <v>794</v>
+        <v>530</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="D5">
+        <v>30</v>
+      </c>
+      <c r="E5">
+        <v>30</v>
+      </c>
+      <c r="F5">
+        <v>30</v>
       </c>
       <c r="G5">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="H5">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="I5">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="J5">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="K5">
-        <v>23</v>
-      </c>
-      <c r="L5" t="s">
-        <v>34</v>
-      </c>
-      <c r="M5" t="s">
-        <v>34</v>
-      </c>
-      <c r="N5" t="s">
-        <v>34</v>
-      </c>
-      <c r="O5" t="s">
-        <v>34</v>
+        <v>30</v>
+      </c>
+      <c r="L5">
+        <v>30</v>
+      </c>
+      <c r="M5">
+        <v>30</v>
+      </c>
+      <c r="N5">
+        <v>30</v>
+      </c>
+      <c r="O5">
+        <v>30</v>
       </c>
       <c r="P5">
-        <v>119</v>
+        <v>360</v>
       </c>
       <c r="Q5">
-        <v>913</v>
+        <v>890</v>
       </c>
       <c r="R5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="S5" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" s="3" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="B6">
-        <v>889</v>
+        <v>794</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6">
-        <v>12</v>
-      </c>
-      <c r="E6">
-        <v>13</v>
-      </c>
-      <c r="F6">
-        <v>13</v>
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" t="s">
+        <v>35</v>
       </c>
       <c r="G6">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="H6">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="I6">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="J6">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K6">
-        <v>12</v>
-      </c>
-      <c r="L6">
-        <v>12</v>
+        <v>23</v>
+      </c>
+      <c r="L6" t="s">
+        <v>35</v>
       </c>
       <c r="M6" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="N6" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="O6" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="P6">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="Q6">
-        <v>1000</v>
+        <v>913</v>
       </c>
       <c r="R6" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="S6" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -1768,58 +1773,58 @@
         <v>48</v>
       </c>
       <c r="B7">
-        <v>1500</v>
+        <v>889</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" t="s">
-        <v>53</v>
+        <v>33</v>
+      </c>
+      <c r="D7">
+        <v>12</v>
+      </c>
+      <c r="E7">
+        <v>13</v>
+      </c>
+      <c r="F7">
+        <v>13</v>
       </c>
       <c r="G7">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H7">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="I7">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J7">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="K7">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="L7">
-        <v>9</v>
-      </c>
-      <c r="M7">
-        <v>9</v>
-      </c>
-      <c r="N7">
-        <v>9</v>
-      </c>
-      <c r="O7">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="M7" t="s">
+        <v>56</v>
+      </c>
+      <c r="N7" t="s">
+        <v>56</v>
+      </c>
+      <c r="O7" t="s">
+        <v>56</v>
       </c>
       <c r="P7">
-        <v>80</v>
+        <v>111</v>
       </c>
       <c r="Q7">
-        <v>1580</v>
+        <v>1000</v>
       </c>
       <c r="R7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -1827,249 +1832,299 @@
         <v>49</v>
       </c>
       <c r="B8">
-        <v>1697</v>
+        <v>1500</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8">
-        <v>30</v>
-      </c>
-      <c r="E8">
-        <v>30</v>
-      </c>
-      <c r="F8">
-        <v>30</v>
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" t="s">
+        <v>54</v>
       </c>
       <c r="G8">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="H8">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="I8">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="J8">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="K8">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="L8">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="M8">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="N8">
-        <v>23</v>
-      </c>
-      <c r="O8" t="s">
-        <v>57</v>
+        <v>9</v>
+      </c>
+      <c r="O8">
+        <v>9</v>
       </c>
       <c r="P8">
-        <v>303</v>
+        <v>80</v>
       </c>
       <c r="Q8">
-        <v>2000</v>
+        <v>1580</v>
       </c>
       <c r="R8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B9" t="s">
-        <v>52</v>
+      <c r="B9">
+        <v>1697</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D9">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="E9">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="F9">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="G9">
-        <v>18</v>
-      </c>
-      <c r="H9" t="s">
-        <v>34</v>
-      </c>
-      <c r="I9" t="s">
-        <v>34</v>
-      </c>
-      <c r="J9" t="s">
-        <v>34</v>
-      </c>
-      <c r="K9" t="s">
-        <v>34</v>
-      </c>
-      <c r="L9" t="s">
-        <v>55</v>
-      </c>
-      <c r="M9" t="s">
-        <v>55</v>
-      </c>
-      <c r="N9" t="s">
-        <v>55</v>
+        <v>30</v>
+      </c>
+      <c r="H9">
+        <v>29</v>
+      </c>
+      <c r="I9">
+        <v>28</v>
+      </c>
+      <c r="J9">
+        <v>27</v>
+      </c>
+      <c r="K9">
+        <v>26</v>
+      </c>
+      <c r="L9">
+        <v>26</v>
+      </c>
+      <c r="M9">
+        <v>24</v>
+      </c>
+      <c r="N9">
+        <v>23</v>
       </c>
       <c r="O9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="P9">
-        <v>70</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>58</v>
+        <v>303</v>
+      </c>
+      <c r="Q9">
+        <v>2000</v>
       </c>
       <c r="R9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S9" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B10">
-        <v>1447</v>
+      <c r="B10" t="s">
+        <v>53</v>
       </c>
       <c r="C10" t="s">
         <v>33</v>
       </c>
       <c r="D10">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="E10">
-        <v>23</v>
-      </c>
-      <c r="F10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G10" t="s">
-        <v>54</v>
+        <v>17</v>
+      </c>
+      <c r="F10">
+        <v>18</v>
+      </c>
+      <c r="G10">
+        <v>18</v>
       </c>
       <c r="H10" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="I10" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="J10" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="K10" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="L10">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="M10">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="N10">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="O10">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="P10">
-        <v>173</v>
-      </c>
-      <c r="Q10">
-        <v>1620</v>
+        <v>130</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>58</v>
       </c>
       <c r="R10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S10" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11">
+        <v>1447</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11">
+        <v>30</v>
+      </c>
+      <c r="E11">
+        <v>23</v>
+      </c>
+      <c r="F11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" t="s">
+        <v>55</v>
+      </c>
+      <c r="J11" t="s">
+        <v>55</v>
+      </c>
+      <c r="K11" t="s">
+        <v>55</v>
+      </c>
+      <c r="L11">
+        <v>30</v>
+      </c>
+      <c r="M11">
+        <v>30</v>
+      </c>
+      <c r="N11">
+        <v>30</v>
+      </c>
+      <c r="O11">
+        <v>30</v>
+      </c>
+      <c r="P11">
+        <v>173</v>
+      </c>
+      <c r="Q11">
+        <v>1620</v>
+      </c>
+      <c r="R11" t="s">
+        <v>35</v>
+      </c>
+      <c r="S11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="A12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>2000</v>
       </c>
-      <c r="C11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="C12" t="s">
         <v>34</v>
       </c>
-      <c r="E11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H11" t="s">
-        <v>34</v>
-      </c>
-      <c r="I11">
+      <c r="D12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12">
         <v>27</v>
       </c>
-      <c r="J11">
+      <c r="J12">
         <v>25</v>
       </c>
-      <c r="K11">
+      <c r="K12">
         <v>25</v>
       </c>
-      <c r="L11" t="s">
-        <v>34</v>
-      </c>
-      <c r="M11" t="s">
-        <v>34</v>
-      </c>
-      <c r="N11" t="s">
-        <v>34</v>
-      </c>
-      <c r="O11" t="s">
-        <v>34</v>
-      </c>
-      <c r="P11">
+      <c r="L12" t="s">
+        <v>35</v>
+      </c>
+      <c r="M12" t="s">
+        <v>35</v>
+      </c>
+      <c r="N12" t="s">
+        <v>35</v>
+      </c>
+      <c r="O12" t="s">
+        <v>35</v>
+      </c>
+      <c r="P12">
         <v>77</v>
       </c>
-      <c r="Q11">
+      <c r="Q12">
         <v>2077</v>
       </c>
-      <c r="R11" t="s">
+      <c r="R12" t="s">
         <v>59</v>
       </c>
-      <c r="S11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19">
-      <c r="P13" s="4">
-        <f>SUM(P3:P11)</f>
-        <v>0</v>
-      </c>
-      <c r="R13" s="4" t="s">
-        <v>43</v>
+      <c r="S12" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:19">
       <c r="P14" s="4">
-        <v>1043</v>
+        <v>1442</v>
       </c>
       <c r="R14" s="4" t="s">
         <v>44</v>
@@ -2077,10 +2132,18 @@
     </row>
     <row r="15" spans="1:19">
       <c r="P15" s="4">
-        <v>250</v>
+        <v>1192</v>
       </c>
       <c r="R15" s="4" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="P16" s="4">
+        <v>250</v>
+      </c>
+      <c r="R16" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -2102,7 +2165,7 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="G1" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -2113,7 +2176,7 @@
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2"/>
     </row>
@@ -2184,31 +2247,31 @@
         <v>375</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L4">
         <v>30</v>
@@ -2232,7 +2295,7 @@
         <v>59</v>
       </c>
       <c r="S4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -2243,7 +2306,7 @@
         <v>340</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D5">
         <v>27</v>
@@ -2267,19 +2330,19 @@
         <v>17</v>
       </c>
       <c r="K5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="P5">
         <v>160</v>
@@ -2288,10 +2351,10 @@
         <v>500</v>
       </c>
       <c r="R5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -2302,7 +2365,7 @@
         <v>719</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D6">
         <v>25</v>
@@ -2314,31 +2377,31 @@
         <v>25</v>
       </c>
       <c r="G6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="O6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P6">
         <v>75</v>
@@ -2347,10 +2410,10 @@
         <v>794</v>
       </c>
       <c r="R6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -2361,7 +2424,7 @@
         <v>1000</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
         <v>64</v>
@@ -2406,10 +2469,10 @@
         <v>1108</v>
       </c>
       <c r="R7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -2420,7 +2483,7 @@
         <v>1338</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D8">
         <v>14</v>
@@ -2456,7 +2519,7 @@
         <v>15</v>
       </c>
       <c r="O8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="P8">
         <v>162</v>
@@ -2465,10 +2528,10 @@
         <v>1500</v>
       </c>
       <c r="R8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -2479,22 +2542,22 @@
         <v>1666</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I9">
         <v>11</v>
@@ -2509,13 +2572,13 @@
         <v>10</v>
       </c>
       <c r="M9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="O9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P9">
         <v>41</v>
@@ -2527,54 +2590,54 @@
         <v>59</v>
       </c>
       <c r="S9" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B10">
         <v>1850</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H10" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="I10" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="J10" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="K10" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="L10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="O10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P10">
         <v>0</v>
@@ -2583,10 +2646,10 @@
         <v>1850</v>
       </c>
       <c r="R10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="S10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:19">
@@ -2597,31 +2660,31 @@
         <v>2077</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L11">
         <v>27</v>
@@ -2642,19 +2705,18 @@
         <v>2177</v>
       </c>
       <c r="R11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="S11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:19">
       <c r="P13" s="4">
-        <f>SUM(P3:P11)</f>
-        <v>0</v>
+        <v>766</v>
       </c>
       <c r="R13" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:19">
@@ -2662,7 +2724,7 @@
         <v>666</v>
       </c>
       <c r="R14" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:19">
@@ -2670,7 +2732,7 @@
         <v>100</v>
       </c>
       <c r="R15" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -2684,7 +2746,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S12"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2692,7 +2754,7 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="G1" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -2703,7 +2765,7 @@
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2"/>
     </row>
@@ -2768,322 +2830,262 @@
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="3" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="B4">
-        <v>322</v>
+        <v>242</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" t="s">
-        <v>34</v>
-      </c>
-      <c r="J4" t="s">
-        <v>34</v>
-      </c>
-      <c r="K4" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="D4">
+        <v>30</v>
+      </c>
+      <c r="E4">
+        <v>30</v>
+      </c>
+      <c r="F4">
+        <v>30</v>
+      </c>
+      <c r="G4">
+        <v>30</v>
+      </c>
+      <c r="H4">
+        <v>30</v>
+      </c>
+      <c r="I4">
+        <v>30</v>
+      </c>
+      <c r="J4">
+        <v>28</v>
+      </c>
+      <c r="K4">
+        <v>26</v>
       </c>
       <c r="L4">
-        <v>27</v>
-      </c>
-      <c r="M4">
-        <v>26</v>
-      </c>
-      <c r="N4">
         <v>24</v>
       </c>
-      <c r="O4">
-        <v>23</v>
+      <c r="M4" t="s">
+        <v>74</v>
+      </c>
+      <c r="N4" t="s">
+        <v>74</v>
+      </c>
+      <c r="O4" t="s">
+        <v>74</v>
       </c>
       <c r="P4">
-        <v>100</v>
+        <v>258</v>
       </c>
       <c r="Q4">
-        <v>422</v>
+        <v>500</v>
       </c>
       <c r="R4" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="S4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B5">
-        <v>242</v>
+        <v>500</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5">
-        <v>30</v>
-      </c>
-      <c r="E5">
-        <v>30</v>
-      </c>
-      <c r="F5">
-        <v>30</v>
-      </c>
-      <c r="G5">
-        <v>30</v>
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" t="s">
+        <v>73</v>
       </c>
       <c r="H5">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I5">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="J5">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="K5">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L5">
         <v>24</v>
       </c>
-      <c r="M5" t="s">
-        <v>72</v>
-      </c>
-      <c r="N5" t="s">
-        <v>72</v>
-      </c>
-      <c r="O5" t="s">
-        <v>72</v>
+      <c r="M5">
+        <v>23</v>
+      </c>
+      <c r="N5">
+        <v>21</v>
+      </c>
+      <c r="O5">
+        <v>21</v>
       </c>
       <c r="P5">
-        <v>258</v>
+        <v>192</v>
       </c>
       <c r="Q5">
-        <v>500</v>
+        <v>692</v>
       </c>
       <c r="R5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" s="3" t="s">
-        <v>69</v>
+        <v>24</v>
       </c>
       <c r="B6">
-        <v>500</v>
+        <v>1707</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="F6" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="G6" t="s">
-        <v>71</v>
-      </c>
-      <c r="H6">
-        <v>27</v>
-      </c>
-      <c r="I6">
-        <v>26</v>
-      </c>
-      <c r="J6">
-        <v>25</v>
-      </c>
-      <c r="K6">
-        <v>25</v>
-      </c>
-      <c r="L6">
-        <v>24</v>
+        <v>35</v>
+      </c>
+      <c r="H6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" t="s">
+        <v>35</v>
       </c>
       <c r="M6">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="N6">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="O6">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="P6">
-        <v>192</v>
+        <v>29</v>
       </c>
       <c r="Q6">
-        <v>692</v>
+        <v>1736</v>
       </c>
       <c r="R6" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="S6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="3" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="B7">
-        <v>1707</v>
+        <v>531</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" t="s">
         <v>34</v>
       </c>
-      <c r="E7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" t="s">
-        <v>34</v>
-      </c>
-      <c r="I7" t="s">
-        <v>34</v>
-      </c>
-      <c r="J7" t="s">
-        <v>34</v>
-      </c>
-      <c r="K7" t="s">
-        <v>34</v>
-      </c>
-      <c r="L7" t="s">
-        <v>34</v>
+      <c r="D7">
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <v>8</v>
+      </c>
+      <c r="F7">
+        <v>9</v>
+      </c>
+      <c r="G7">
+        <v>9</v>
+      </c>
+      <c r="H7">
+        <v>9</v>
+      </c>
+      <c r="I7">
+        <v>9</v>
+      </c>
+      <c r="J7">
+        <v>8</v>
+      </c>
+      <c r="K7">
+        <v>8</v>
+      </c>
+      <c r="L7">
+        <v>8</v>
       </c>
       <c r="M7">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="N7">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="O7">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P7">
-        <v>29</v>
+        <v>100</v>
       </c>
       <c r="Q7">
-        <v>1736</v>
+        <v>631</v>
       </c>
       <c r="R7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="S7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19">
-      <c r="A8" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B8">
-        <v>531</v>
-      </c>
-      <c r="C8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8">
-        <v>8</v>
-      </c>
-      <c r="E8">
-        <v>8</v>
-      </c>
-      <c r="F8">
-        <v>9</v>
-      </c>
-      <c r="G8">
-        <v>9</v>
-      </c>
-      <c r="H8">
-        <v>9</v>
-      </c>
-      <c r="I8">
-        <v>9</v>
-      </c>
-      <c r="J8">
-        <v>8</v>
-      </c>
-      <c r="K8">
-        <v>8</v>
-      </c>
-      <c r="L8">
-        <v>8</v>
-      </c>
-      <c r="M8">
-        <v>8</v>
-      </c>
-      <c r="N8">
-        <v>8</v>
-      </c>
-      <c r="O8">
-        <v>8</v>
-      </c>
-      <c r="P8">
-        <v>100</v>
-      </c>
-      <c r="Q8">
-        <v>631</v>
-      </c>
-      <c r="R8" t="s">
-        <v>34</v>
-      </c>
-      <c r="S8" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="P9" s="4">
+        <v>579</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:19">
       <c r="P10" s="4">
-        <f>SUM(P3:P8)</f>
-        <v>0</v>
+        <v>479</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:19">
       <c r="P11" s="4">
-        <v>579</v>
+        <v>100</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19">
-      <c r="P12" s="4">
-        <v>100</v>
-      </c>
-      <c r="R12" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>